<commit_message>
Corrección a 8 desarrolladores
Co  8 desarrolladores nuestro punto función nos arroja un tiempo de 6 meses para realizar el proyecto.
</commit_message>
<xml_diff>
--- a/Punto Funcion.xlsx
+++ b/Punto Funcion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\GitHub\PROYECTO-IS-II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\PROYECTO-IS-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22230" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="22236" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -792,22 +792,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -839,7 +839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>27</v>
       </c>
@@ -865,7 +865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -993,7 +993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>71</v>
       </c>
@@ -1089,10 +1089,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>56</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>19</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>20</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>21</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>26</v>
       </c>
@@ -1384,13 +1384,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>6</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>13</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1544,42 +1544,42 @@
         <v>4659.2000000000007</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41">
         <f>B39/B40</f>
-        <v>202.57391304347829</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>582.40000000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="B42">
         <f>B41/5</f>
-        <v>40.514782608695654</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116.48000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43">
         <f>B42/20</f>
-        <v>2.0257391304347827</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.8240000000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1587,12 +1587,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>60</v>
       </c>
@@ -1600,12 +1600,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>62</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>63</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>67</v>
       </c>
@@ -1629,16 +1629,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>66</v>
       </c>
       <c r="D58">
         <f>SUM(D48:D52) *B43</f>
-        <v>1418.0173913043479</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4076.8000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>47</v>
       </c>
@@ -1648,14 +1648,14 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11">
         <f>(B40*B43*B45)+D58</f>
-        <v>24714.017391304347</v>
+        <v>27372.800000000003</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>64</v>
       </c>
@@ -1663,32 +1663,32 @@
         <v>600</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>69</v>
       </c>
       <c r="D62">
         <f>D60*0.01</f>
-        <v>247.14017391304347</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>273.72800000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>65</v>
       </c>
       <c r="D63">
         <f>D60*(0.05)</f>
-        <v>1235.7008695652175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1368.6400000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10">
         <f>SUM(D60:D63)</f>
-        <v>26796.858434782611</v>
+        <v>29615.168000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>